<commit_message>
Revert "Revert "엑셀 데이터 추가""
This reverts commit 5f678c9b69d0eba5d39106dcf11a870381450a30.
</commit_message>
<xml_diff>
--- a/Design/Excel/CharacterStatTable.xlsx
+++ b/Design/Excel/CharacterStatTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ProjectSD_Master\Common\ExcelDatas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ProjectPM\Design\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FC8E5C-434D-4EC0-85B6-384D39912A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40792F40-5327-499D-B7E7-2FDF6898FCBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6532FEE8-E746-4D08-A68F-0FB7B4F7089F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6532FEE8-E746-4D08-A68F-0FB7B4F7089F}"/>
   </bookViews>
   <sheets>
     <sheet name="CharacterStat" sheetId="1" r:id="rId1"/>
@@ -34,53 +34,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t># 0 : Solider</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Strength</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Intelligence</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Health</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mentality</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PhysicalAttack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MagicalAttack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HpMax</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MpMax</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t># ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#1 : Blue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#0 : Red</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#2 : Green</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#3 : Black</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jumpPower</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>moveSpeed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attackSpeed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -445,23 +441,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67048CF9-92A1-40E0-A99C-FF7E174B99E8}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.796875" customWidth="1"/>
-    <col min="2" max="2" width="13.296875" customWidth="1"/>
-    <col min="3" max="3" width="13.3984375" customWidth="1"/>
+    <col min="1" max="1" width="12.75" customWidth="1"/>
+    <col min="2" max="2" width="13.25" customWidth="1"/>
+    <col min="3" max="3" width="13.375" customWidth="1"/>
     <col min="4" max="4" width="12.5" customWidth="1"/>
-    <col min="5" max="6" width="16.09765625" customWidth="1"/>
-    <col min="7" max="7" width="10.8984375" customWidth="1"/>
+    <col min="5" max="6" width="16.125" customWidth="1"/>
+    <col min="7" max="7" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -477,85 +473,115 @@
       <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="C3">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="D3">
-        <v>150</v>
+        <v>8</v>
       </c>
       <c r="E3">
-        <v>100</v>
-      </c>
-      <c r="F3">
-        <v>250</v>
-      </c>
-      <c r="G3">
-        <v>20</v>
-      </c>
-      <c r="H3">
-        <v>500</v>
-      </c>
-      <c r="I3">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>1</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>